<commit_message>
ajuste tempo carremento consulta
</commit_message>
<xml_diff>
--- a/02_coleta_temp/coleta_temp.xlsx
+++ b/02_coleta_temp/coleta_temp.xlsx
@@ -454,7 +454,7 @@
       <c r="B2" t="inlineStr">
         <is>
           <t xml:space="preserve">Consulta Optantes
-Data da consulta: 30/04/2024 11:12:18
+Data da consulta: 30/04/2024 11:19:18
 Identificação do Contribuinte - CNPJ Matriz
 CNPJ: 33.657.248/0001-89
 A opção pelo Simples Nacional e/ou SIMEI abrange todos os estabelecimentos da empresa
@@ -475,7 +475,7 @@
       <c r="B3" t="inlineStr">
         <is>
           <t xml:space="preserve">Consulta Optantes
-Data da consulta: 30/04/2024 11:12:22
+Data da consulta: 30/04/2024 11:19:22
 Identificação do Contribuinte - CNPJ Matriz
 CNPJ: 90.400.888/0001-42
 A opção pelo Simples Nacional e/ou SIMEI abrange todos os estabelecimentos da empresa

</xml_diff>